<commit_message>
update if blank KC
</commit_message>
<xml_diff>
--- a/data_demo/A.xlsx
+++ b/data_demo/A.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dungnguyen/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dungnguyen/Desktop/Data Science off/Python Programming/1. Work Project/21_san_xuat_stat/data_demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B046CC-9E1F-8642-A3BA-B1E37401A87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263AE194-0EC8-5A4F-A7A7-BF51BFAF74BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>Danh sách câu hỏi thuộc ngân hàng "Test câu hỏi" - 16572258</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>Bạn nghĩ như thế nào là kinh doanh?</t>
-  </si>
-  <si>
-    <t>03.K6.1.5.1 - Nhận biết được số đối của một phân số.|03.K6.1.6.1 - Nhận biết được hỗn số dương</t>
   </si>
 </sst>
 </file>
@@ -227,10 +224,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,7 +535,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -554,40 +551,40 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -849,9 +846,7 @@
       <c r="G11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1">
         <v>1</v>
@@ -866,6 +861,11 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="12">
+    <mergeCell ref="A3"/>
+    <mergeCell ref="B3"/>
+    <mergeCell ref="C3"/>
+    <mergeCell ref="D3"/>
+    <mergeCell ref="E3"/>
     <mergeCell ref="K3"/>
     <mergeCell ref="L3"/>
     <mergeCell ref="F3"/>
@@ -873,11 +873,6 @@
     <mergeCell ref="H3"/>
     <mergeCell ref="I3"/>
     <mergeCell ref="J3"/>
-    <mergeCell ref="A3"/>
-    <mergeCell ref="B3"/>
-    <mergeCell ref="C3"/>
-    <mergeCell ref="D3"/>
-    <mergeCell ref="E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>